<commit_message>
Added new item to risk assessment
</commit_message>
<xml_diff>
--- a/risk_assessment/DCPP-risk-assessment.xlsx
+++ b/risk_assessment/DCPP-risk-assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\QA\Practical Project 2\dcpp\risk_assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0913B1EE-48EA-40F8-BA11-E34C4FB1F08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57438D4-44D5-43FA-9F14-76CAA66DBCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4785" yWindow="6090" windowWidth="24780" windowHeight="12390" xr2:uid="{2EFD2869-BFFC-4FAF-877A-2E81F4DE0D36}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>SEVERITY</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>Ensure delivery is secured from external attack</t>
+  </si>
+  <si>
+    <t>Not enough time alloted to complete the task</t>
+  </si>
+  <si>
+    <t>Lack of Time</t>
+  </si>
+  <si>
+    <t>Extend time allocation</t>
+  </si>
+  <si>
+    <t>To fully complete the task</t>
   </si>
 </sst>
 </file>
@@ -223,7 +235,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,13 +932,27 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="15"/>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="15">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -951,18 +977,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1098,18 +1124,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{888C558A-737D-4AB2-A5CF-DEA79ED69469}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68AF4FA-6C86-4C24-9AB0-65AD4D282361}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68AF4FA-6C86-4C24-9AB0-65AD4D282361}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{888C558A-737D-4AB2-A5CF-DEA79ED69469}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>